<commit_message>
feat:tratamento de campos vazios
</commit_message>
<xml_diff>
--- a/Automação de Mensagens WhatsApp/Contatos.xlsx
+++ b/Automação de Mensagens WhatsApp/Contatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Area de Trabalho\Desktop\Danilo TI\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255D538A-BE81-4521-9479-DE0715025928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E442DE-C614-485F-AB71-7C1DDB0F32CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{84EF6E06-1BA5-48F0-B452-529FC31460B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>Mensagem</t>
   </si>
@@ -49,13 +49,24 @@
   <si>
     <t>E:\Area de Trabalho\Desktop\Danilo TI\álbuns galeria\Capas\Reuniões 2023\1.jpeg</t>
   </si>
+  <si>
+    <t>61998232332</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -83,8 +94,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,20 +412,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D646578E-F6F4-40C8-847F-93B464363753}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="1" max="1" width="61" style="1" customWidth="1"/>
     <col min="2" max="2" width="108.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
@@ -420,30 +433,47 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>5561998232332</v>
+      <c r="A2" s="1">
+        <v>61998232332</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>5561998232332</v>
+      <c r="A3" s="1">
+        <v>61998232332</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5561998232332</v>
+      <c r="A4" s="1">
+        <v>61998232332</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>